<commit_message>
Read stuff better and fix lin regression
</commit_message>
<xml_diff>
--- a/data/Bacteria_data.xlsx
+++ b/data/Bacteria_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eseitar\Desktop\courses\Phy212\Projects\Module 3\Ilya's projects data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mack/Documents/Physics212/bacteria/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991D8230-6596-984E-AD8E-53450F4FBC7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12060" windowHeight="6960"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12060" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,11 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -349,200 +357,200 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A52"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>4</v>
       </c>
       <c r="B2" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>5</v>
       </c>
       <c r="B4" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>6</v>
       </c>
       <c r="B6" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
         <v>330</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="2">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2">
         <v>820</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2">
-        <v>8840</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="2">
-        <v>3880</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8840</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>11</v>
       </c>
       <c r="B15" s="2">
+        <v>3880</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>11</v>
+      </c>
+      <c r="B16" s="2">
         <v>3700</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>13.03</v>
-      </c>
-      <c r="B16" s="2">
-        <v>155000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>13.03</v>
       </c>
       <c r="B17" s="2">
-        <v>17700</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>155000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>13.03</v>
       </c>
       <c r="B18" s="2">
+        <v>17700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>13.03</v>
+      </c>
+      <c r="B19" s="2">
         <v>19000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>14.56</v>
-      </c>
-      <c r="B19" s="2">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>14.56</v>
       </c>
       <c r="B20" s="2">
-        <v>87000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>14.56</v>
       </c>
       <c r="B21" s="2">
+        <v>87000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>14.56</v>
+      </c>
+      <c r="B22" s="2">
         <v>70400</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>18.22</v>
-      </c>
-      <c r="B22" s="2">
-        <v>310000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>18.22</v>
       </c>
       <c r="B23" s="2">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>310000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>18.22</v>
       </c>
@@ -550,227 +558,235 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>18.22</v>
       </c>
       <c r="B25" s="2">
-        <v>55000000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" s="2">
-        <v>42000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" s="2">
+        <v>42000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2">
         <v>55000000</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>22</v>
-      </c>
-      <c r="B28" s="2">
-        <v>42600000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>22</v>
       </c>
       <c r="B29" s="2">
+        <v>42600000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>22</v>
+      </c>
+      <c r="B30" s="2">
         <v>113000000</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>24</v>
-      </c>
-      <c r="B30" s="2">
-        <v>75800000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>24</v>
       </c>
       <c r="B31" s="2">
+        <v>75800000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>24</v>
+      </c>
+      <c r="B32" s="2">
         <v>126000000</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="B32" s="2">
-        <v>153000000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>25.5</v>
       </c>
       <c r="B33" s="2">
+        <v>153000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="B34" s="2">
         <v>79500000</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>35</v>
-      </c>
-      <c r="B34" s="2">
-        <v>99500000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>35</v>
       </c>
       <c r="B35" s="2">
+        <v>99500000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
         <v>119000000</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>38</v>
-      </c>
-      <c r="B36" s="2">
-        <v>53200000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>38</v>
       </c>
       <c r="B37" s="2">
+        <v>53200000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>38</v>
+      </c>
+      <c r="B38" s="2">
         <v>198000000</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>41</v>
-      </c>
-      <c r="B38" s="2">
-        <v>80200000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>41</v>
       </c>
       <c r="B39" s="2">
+        <v>80200000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>41</v>
+      </c>
+      <c r="B40" s="2">
         <v>129000000</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
         <v>60</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B41" s="2">
         <v>117000000</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>64</v>
-      </c>
-      <c r="B41" s="2">
-        <v>114000000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>64</v>
       </c>
       <c r="B42" s="2">
+        <v>114000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>64</v>
+      </c>
+      <c r="B43" s="2">
         <v>97000000</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>78</v>
-      </c>
-      <c r="B43" s="2">
-        <v>95000000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>78</v>
       </c>
       <c r="B44" s="2">
+        <v>95000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>78</v>
+      </c>
+      <c r="B45" s="2">
         <v>79000000</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>100</v>
-      </c>
-      <c r="B45" s="2">
-        <v>94400000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>100</v>
       </c>
       <c r="B46" s="2">
+        <v>94400000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>100</v>
+      </c>
+      <c r="B47" s="2">
         <v>89500000</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>6</v>
-      </c>
-      <c r="B47" s="2">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>6</v>
       </c>
       <c r="B48" s="2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>6</v>
+      </c>
+      <c r="B49" s="2">
         <v>290</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>7</v>
-      </c>
-      <c r="B49" s="2">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>7</v>
       </c>
       <c r="B50" s="2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>7</v>
+      </c>
+      <c r="B51" s="2">
         <v>590</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>8</v>
-      </c>
-      <c r="B51" s="2">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>8</v>
       </c>
       <c r="B52" s="2">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>8</v>
+      </c>
+      <c r="B53" s="2">
         <v>680</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Got K and a
</commit_message>
<xml_diff>
--- a/data/Bacteria_data.xlsx
+++ b/data/Bacteria_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mack/Documents/Physics212/bacteria/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991D8230-6596-984E-AD8E-53450F4FBC7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA12BF59-A284-EF41-9ABC-2545A2590BE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12060" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18200" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -361,7 +361,7 @@
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -424,373 +424,376 @@
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2">
-        <v>245</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2">
-        <v>365</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2">
-        <v>330</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2">
-        <v>785</v>
+        <v>440</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2">
-        <v>820</v>
+        <v>590</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2">
-        <v>8840</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2">
-        <v>3880</v>
+        <v>330</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2">
-        <v>3700</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>13.03</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2">
-        <v>155000</v>
+        <v>680</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>13.03</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2">
-        <v>17700</v>
+        <v>785</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>13.03</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2">
-        <v>19000</v>
+        <v>820</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>14.56</v>
+        <v>11</v>
       </c>
       <c r="B20" s="2">
-        <v>30000</v>
+        <v>8840</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>14.56</v>
+        <v>11</v>
       </c>
       <c r="B21" s="2">
-        <v>87000</v>
+        <v>3880</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>14.56</v>
+        <v>11</v>
       </c>
       <c r="B22" s="2">
-        <v>70400</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>18.22</v>
+        <v>13.03</v>
       </c>
       <c r="B23" s="2">
-        <v>310000</v>
+        <v>155000</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>18.22</v>
+        <v>13.03</v>
       </c>
       <c r="B24" s="2">
-        <v>500000</v>
+        <v>17700</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>18.22</v>
+        <v>13.03</v>
       </c>
       <c r="B25" s="2">
-        <v>500000</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>14.56</v>
       </c>
       <c r="B26" s="2">
-        <v>55000000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>24</v>
+        <v>14.56</v>
       </c>
       <c r="B27" s="2">
-        <v>42000000</v>
+        <v>87000</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>24</v>
+        <v>14.56</v>
       </c>
       <c r="B28" s="2">
-        <v>55000000</v>
+        <v>70400</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>22</v>
+        <v>18.22</v>
       </c>
       <c r="B29" s="2">
-        <v>42600000</v>
+        <v>310000</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>22</v>
+        <v>18.22</v>
       </c>
       <c r="B30" s="2">
-        <v>113000000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>24</v>
+        <v>18.22</v>
       </c>
       <c r="B31" s="2">
-        <v>75800000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32" s="2">
-        <v>126000000</v>
+        <v>42600000</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>25.5</v>
+        <v>22</v>
       </c>
       <c r="B33" s="2">
-        <v>153000000</v>
+        <v>113000000</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>25.5</v>
+        <v>24</v>
       </c>
       <c r="B34" s="2">
-        <v>79500000</v>
+        <v>55000000</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B35" s="2">
-        <v>99500000</v>
+        <v>42000000</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B36" s="2">
-        <v>119000000</v>
+        <v>55000000</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B37" s="2">
-        <v>53200000</v>
+        <v>75800000</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B38" s="2">
-        <v>198000000</v>
+        <v>126000000</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>41</v>
+        <v>25.5</v>
       </c>
       <c r="B39" s="2">
-        <v>80200000</v>
+        <v>153000000</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>41</v>
+        <v>25.5</v>
       </c>
       <c r="B40" s="2">
-        <v>129000000</v>
+        <v>79500000</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B41" s="2">
-        <v>117000000</v>
+        <v>99500000</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="B42" s="2">
-        <v>114000000</v>
+        <v>119000000</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="B43" s="2">
-        <v>97000000</v>
+        <v>53200000</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="B44" s="2">
-        <v>95000000</v>
+        <v>198000000</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="B45" s="2">
-        <v>79000000</v>
+        <v>80200000</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="B46" s="2">
-        <v>94400000</v>
+        <v>129000000</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="B47" s="2">
-        <v>89500000</v>
+        <v>117000000</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B48" s="2">
-        <v>240</v>
+        <v>114000000</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B49" s="2">
-        <v>290</v>
+        <v>97000000</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="B50" s="2">
-        <v>440</v>
+        <v>95000000</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="B51" s="2">
-        <v>590</v>
+        <v>79000000</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="B52" s="2">
-        <v>1290</v>
+        <v>94400000</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="B53" s="2">
-        <v>680</v>
+        <v>89500000</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B53">
+    <sortCondition ref="A2:A53"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>